<commit_message>
updated English country data books added.
</commit_message>
<xml_diff>
--- a/inputs/en/LiST countries/Afghanistan_databook.xlsx
+++ b/inputs/en/LiST countries/Afghanistan_databook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="2" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Baseline year population inputs" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,29 +11,29 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Causes of death" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nutritional status distribution" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Breastfeeding distribution" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time trends" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time trends" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Economic loss" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IYCF packages" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Treatment of SAM" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs cost and coverage" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Program dependencies" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reference programs" sheetId="12" state="hidden" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Incidence of conditions" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs target population" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Incidence of conditions" sheetId="13" state="hidden" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs target population" sheetId="14" state="hidden" r:id="rId14"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cost curve options" sheetId="15" state="hidden" r:id="rId15"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs family planning" sheetId="16" state="hidden" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs impacted population" sheetId="17" state="hidden" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Program risk areas" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Program risk areas" sheetId="18" state="hidden" r:id="rId18"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Population risk areas" sheetId="19" state="hidden" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IYCF odds ratios" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Birth outcome risks" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relative risks" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Odds ratios" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs birth outcomes" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs anaemia" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs wasting" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs for children" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs for PW" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IYCF odds ratios" sheetId="20" state="hidden" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Birth outcome risks" sheetId="21" state="hidden" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relative risks" sheetId="22" state="hidden" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Odds ratios" sheetId="23" state="hidden" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs birth outcomes" sheetId="24" state="hidden" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs anaemia" sheetId="25" state="hidden" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs wasting" sheetId="26" state="hidden" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs for children" sheetId="27" state="hidden" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programs for PW" sheetId="28" state="hidden" r:id="rId28"/>
   </sheets>
   <definedNames>
     <definedName name="abortion" localSheetId="7">'Baseline year population inputs'!$C$38</definedName>
@@ -96,7 +96,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -209,6 +209,12 @@
       <color theme="0" tint="-0.499984740745262"/>
       <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="7">
@@ -341,13 +347,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -581,9 +588,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
@@ -594,22 +598,27 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="6">
+      <alignment horizontal="right"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="4"/>
     <cellStyle name="Comma 2" xfId="5"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1196,16 +1205,16 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="27.6640625" customWidth="1" style="105" min="1" max="1"/>
+    <col width="27.6640625" customWidth="1" style="106" min="1" max="1"/>
     <col width="38.6640625" customWidth="1" style="70" min="2" max="2"/>
-    <col width="14.44140625" customWidth="1" style="105" min="3" max="7"/>
-    <col width="14.44140625" customWidth="1" style="105" min="8" max="16384"/>
+    <col width="14.44140625" customWidth="1" style="106" min="3" max="7"/>
+    <col width="14.44140625" customWidth="1" style="106" min="8" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.9" customHeight="1" s="2">
@@ -1226,7 +1235,7 @@
       </c>
     </row>
     <row r="2" ht="15.9" customHeight="1" s="2">
-      <c r="A2" s="105" t="inlineStr">
+      <c r="A2" s="106" t="inlineStr">
         <is>
           <t>Projection years</t>
         </is>
@@ -1262,7 +1271,7 @@
       <c r="C5" s="21" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1" s="2">
-      <c r="A6" s="105" t="inlineStr">
+      <c r="A6" s="106" t="inlineStr">
         <is>
           <t>Population data</t>
         </is>
@@ -1339,10 +1348,10 @@
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="2">
-      <c r="B14" s="105" t="n"/>
+      <c r="B14" s="106" t="n"/>
     </row>
     <row r="15" ht="15" customHeight="1" s="2">
-      <c r="A15" s="105" t="inlineStr">
+      <c r="A15" s="106" t="inlineStr">
         <is>
           <t>Food</t>
         </is>
@@ -1402,10 +1411,10 @@
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="2">
-      <c r="B21" s="105" t="n"/>
+      <c r="B21" s="106" t="n"/>
     </row>
     <row r="22" ht="15" customHeight="1" s="2">
-      <c r="A22" s="105" t="inlineStr">
+      <c r="A22" s="106" t="inlineStr">
         <is>
           <t>Age distribution of pregnant women</t>
         </is>
@@ -1456,7 +1465,7 @@
       <c r="C27" s="8" t="n"/>
     </row>
     <row r="28" ht="15" customHeight="1" s="2">
-      <c r="A28" s="105" t="inlineStr">
+      <c r="A28" s="106" t="inlineStr">
         <is>
           <t>Birth spacing</t>
         </is>
@@ -1524,7 +1533,7 @@
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="2">
-      <c r="A36" s="105" t="inlineStr">
+      <c r="A36" s="106" t="inlineStr">
         <is>
           <t>Mortality</t>
         </is>
@@ -1537,7 +1546,7 @@
           <t>Neonatal mortality (per 1,000 live births)</t>
         </is>
       </c>
-      <c r="C37" s="100" t="n">
+      <c r="C37" s="99" t="n">
         <v>35.8628812848238</v>
       </c>
     </row>
@@ -1547,7 +1556,7 @@
           <t>Infant mortality (per 1,000 live births)</t>
         </is>
       </c>
-      <c r="C38" s="100" t="n">
+      <c r="C38" s="99" t="n">
         <v>46.5128248805674</v>
       </c>
       <c r="D38" s="6" t="n"/>
@@ -1559,7 +1568,7 @@
           <t>Under 5 mortality (per 1,000 live births)</t>
         </is>
       </c>
-      <c r="C39" s="100" t="n">
+      <c r="C39" s="99" t="n">
         <v>60.2693988605884</v>
       </c>
       <c r="D39" s="6" t="n"/>
@@ -1571,7 +1580,7 @@
           <t>Maternal mortality (per 1,000 live births)</t>
         </is>
       </c>
-      <c r="C40" s="100" t="n">
+      <c r="C40" s="99" t="n">
         <v>638</v>
       </c>
     </row>
@@ -1591,7 +1600,7 @@
           <t>Stillbirths (per 1,000 total births)</t>
         </is>
       </c>
-      <c r="C42" s="100" t="n">
+      <c r="C42" s="99" t="n">
         <v>28.37778068</v>
       </c>
     </row>
@@ -1599,7 +1608,7 @@
       <c r="D43" s="6" t="n"/>
     </row>
     <row r="44" ht="15.75" customHeight="1" s="2">
-      <c r="A44" s="105" t="inlineStr">
+      <c r="A44" s="106" t="inlineStr">
         <is>
           <t>Birth outcome distribution</t>
         </is>
@@ -1656,7 +1665,7 @@
       <c r="D49" s="6" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="2">
-      <c r="A50" s="105" t="inlineStr">
+      <c r="A50" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea incidence</t>
         </is>
@@ -1715,7 +1724,7 @@
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="2">
-      <c r="A57" s="105" t="inlineStr">
+      <c r="A57" s="106" t="inlineStr">
         <is>
           <t>Other risks</t>
         </is>
@@ -1767,12 +1776,13 @@
           <t>Low birth weight</t>
         </is>
       </c>
-      <c r="C62" s="106" t="n"/>
+      <c r="C62" s="103" t="n"/>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="2">
       <c r="A63" s="57" t="n"/>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="NsZwz/lcBX8pbh2WKvlt+w==" formatRows="1" sort="1" spinCount="100000" hashValue="T2w3Aa1PBdwufWrS5zJweogwoOIpItY/jwDhu5bgh8R7vUDkU8zC+lmfLdN4F95BSJoHuoQYfGNXGMPv2MoxzA=="/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
@@ -1788,21 +1798,21 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="56" customWidth="1" style="74" min="1" max="1"/>
-    <col width="20" customWidth="1" style="105" min="2" max="2"/>
-    <col width="20.44140625" customWidth="1" style="105" min="3" max="3"/>
-    <col width="20.109375" customWidth="1" style="105" min="4" max="4"/>
-    <col width="36.33203125" bestFit="1" customWidth="1" style="105" min="5" max="5"/>
-    <col width="23" bestFit="1" customWidth="1" style="105" min="6" max="6"/>
-    <col width="22.6640625" bestFit="1" customWidth="1" style="105" min="7" max="7"/>
-    <col width="14.44140625" customWidth="1" style="105" min="8" max="12"/>
-    <col width="14.44140625" customWidth="1" style="105" min="13" max="16384"/>
+    <col width="20" customWidth="1" style="106" min="2" max="2"/>
+    <col width="20.44140625" customWidth="1" style="106" min="3" max="3"/>
+    <col width="20.109375" customWidth="1" style="106" min="4" max="4"/>
+    <col width="36.33203125" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="23" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="22.6640625" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="14.44140625" customWidth="1" style="106" min="8" max="12"/>
+    <col width="14.44140625" customWidth="1" style="106" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.4" customHeight="1" s="2">
@@ -1962,7 +1972,7 @@
         <v>0.95</v>
       </c>
       <c r="D6" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E6" s="91" t="inlineStr">
         <is>
@@ -1989,7 +1999,7 @@
         <v>0.95</v>
       </c>
       <c r="D7" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E7" s="91" t="inlineStr">
         <is>
@@ -2016,7 +2026,7 @@
         <v>0.95</v>
       </c>
       <c r="D8" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E8" s="91" t="inlineStr">
         <is>
@@ -2043,7 +2053,7 @@
         <v>0.95</v>
       </c>
       <c r="D9" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E9" s="91" t="inlineStr">
         <is>
@@ -2340,7 +2350,7 @@
         <v>0.95</v>
       </c>
       <c r="D20" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E20" s="91" t="inlineStr">
         <is>
@@ -2603,11 +2613,15 @@
           <t>Small quantity lipid-based nutrition supplements</t>
         </is>
       </c>
-      <c r="B30" s="48" t="n"/>
+      <c r="B30" s="48" t="n">
+        <v>0</v>
+      </c>
       <c r="C30" s="48" t="n">
         <v>0.95</v>
       </c>
-      <c r="D30" s="91" t="n"/>
+      <c r="D30" s="91" t="n">
+        <v>99</v>
+      </c>
       <c r="E30" s="91" t="inlineStr">
         <is>
           <t>Linear (constant marginal cost) [default]</t>
@@ -2686,7 +2700,9 @@
       <c r="C33" s="48" t="n">
         <v>0.95</v>
       </c>
-      <c r="D33" s="91" t="n"/>
+      <c r="D33" s="91" t="n">
+        <v>99.98999999999999</v>
+      </c>
       <c r="E33" s="91" t="inlineStr">
         <is>
           <t>Linear (constant marginal cost) [default]</t>
@@ -2711,7 +2727,9 @@
       <c r="C34" s="48" t="n">
         <v>0.95</v>
       </c>
-      <c r="D34" s="91" t="n"/>
+      <c r="D34" s="91" t="n">
+        <v>99.98999999999999</v>
+      </c>
       <c r="E34" s="91" t="inlineStr">
         <is>
           <t>Linear (constant marginal cost) [default]</t>
@@ -2737,7 +2755,7 @@
         <v>0.95</v>
       </c>
       <c r="D35" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E35" s="91" t="inlineStr">
         <is>
@@ -2763,7 +2781,9 @@
       <c r="C36" s="48" t="n">
         <v>0.95</v>
       </c>
-      <c r="D36" s="91" t="n"/>
+      <c r="D36" s="91" t="n">
+        <v>99.98999999999999</v>
+      </c>
       <c r="E36" s="91" t="inlineStr">
         <is>
           <t>Linear (constant marginal cost) [default]</t>
@@ -2789,7 +2809,7 @@
         <v>0.95</v>
       </c>
       <c r="D37" s="91" t="n">
-        <v>999.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="E37" s="91" t="inlineStr">
         <is>
@@ -2858,6 +2878,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="OmhKnnxm/88v3UownuDQdw==" formatRows="1" sort="1" spinCount="100000" hashValue="ryohs0BrXu3y/7KcjotPHBwXGjXtnEIM8hoTAe8ZsvhWWVRHOlspLCIpMc5wHAGYWWmljmb08Mfz1W08DHzsSg=="/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
@@ -2880,10 +2901,10 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col width="53" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
-    <col width="47.88671875" customWidth="1" style="105" min="2" max="2"/>
-    <col width="42.44140625" customWidth="1" style="105" min="3" max="3"/>
-    <col width="11.44140625" customWidth="1" style="105" min="4" max="8"/>
-    <col width="11.44140625" customWidth="1" style="105" min="9" max="16384"/>
+    <col width="47.88671875" customWidth="1" style="106" min="2" max="2"/>
+    <col width="42.44140625" customWidth="1" style="106" min="3" max="3"/>
+    <col width="11.44140625" customWidth="1" style="106" min="4" max="8"/>
+    <col width="11.44140625" customWidth="1" style="106" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3053,9 +3074,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="30.109375" customWidth="1" style="105" min="1" max="1"/>
-    <col width="11.44140625" customWidth="1" style="105" min="2" max="6"/>
-    <col width="11.44140625" customWidth="1" style="105" min="7" max="16384"/>
+    <col width="30.109375" customWidth="1" style="106" min="1" max="1"/>
+    <col width="11.44140625" customWidth="1" style="106" min="2" max="6"/>
+    <col width="11.44140625" customWidth="1" style="106" min="7" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3301,7 +3322,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5176,28 +5197,28 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="105" t="inlineStr">
+      <c r="A1" s="106" t="inlineStr">
         <is>
           <t>Linear (constant marginal cost) [default]</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="105" t="inlineStr">
+      <c r="A2" s="106" t="inlineStr">
         <is>
           <t>Curved with increasing marginal cost</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="105" t="inlineStr">
+      <c r="A3" s="106" t="inlineStr">
         <is>
           <t>Curved with decreasing marginal cost</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="105" t="inlineStr">
+      <c r="A4" s="106" t="inlineStr">
         <is>
           <t>S-shaped (decreasing then increasing marginal cost)</t>
         </is>
@@ -5223,12 +5244,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="33.6640625" customWidth="1" style="105" min="1" max="1"/>
-    <col width="12.44140625" customWidth="1" style="105" min="2" max="2"/>
-    <col width="11.44140625" customWidth="1" style="105" min="3" max="4"/>
-    <col width="17.44140625" customWidth="1" style="105" min="5" max="5"/>
-    <col width="11.44140625" customWidth="1" style="105" min="6" max="10"/>
-    <col width="11.44140625" customWidth="1" style="105" min="11" max="16384"/>
+    <col width="33.6640625" customWidth="1" style="106" min="1" max="1"/>
+    <col width="12.44140625" customWidth="1" style="106" min="2" max="2"/>
+    <col width="11.44140625" customWidth="1" style="106" min="3" max="4"/>
+    <col width="17.44140625" customWidth="1" style="106" min="5" max="5"/>
+    <col width="11.44140625" customWidth="1" style="106" min="6" max="10"/>
+    <col width="11.44140625" customWidth="1" style="106" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5258,7 +5279,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="13.8" customHeight="1" s="2">
+    <row r="2" ht="13.95" customHeight="1" s="2">
       <c r="A2" s="20" t="inlineStr">
         <is>
           <t>Condom</t>
@@ -5267,18 +5288,18 @@
       <c r="B2" s="20" t="n">
         <v>0.9</v>
       </c>
-      <c r="C2" s="105" t="n">
+      <c r="C2" s="106" t="n">
         <v>0.09</v>
       </c>
-      <c r="D2" s="105" t="n">
+      <c r="D2" s="106" t="n">
         <v>0.8</v>
       </c>
-      <c r="E2" s="105">
+      <c r="E2" s="106">
         <f>C2*D2</f>
         <v/>
       </c>
     </row>
-    <row r="3" ht="13.8" customHeight="1" s="2">
+    <row r="3" ht="13.95" customHeight="1" s="2">
       <c r="A3" s="20" t="inlineStr">
         <is>
           <t>Male sterilization</t>
@@ -5287,18 +5308,18 @@
       <c r="B3" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="105" t="n">
+      <c r="C3" s="106" t="n">
         <v>0.02</v>
       </c>
-      <c r="D3" s="105" t="n">
+      <c r="D3" s="106" t="n">
         <v>1.9</v>
       </c>
-      <c r="E3" s="105">
+      <c r="E3" s="106">
         <f>C3*D3</f>
         <v/>
       </c>
     </row>
-    <row r="4" ht="13.8" customHeight="1" s="2">
+    <row r="4" ht="13.95" customHeight="1" s="2">
       <c r="A4" s="20" t="inlineStr">
         <is>
           <t>Female sterilization</t>
@@ -5307,18 +5328,18 @@
       <c r="B4" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="105" t="n">
+      <c r="C4" s="106" t="n">
         <v>0.08</v>
       </c>
-      <c r="D4" s="105" t="n">
+      <c r="D4" s="106" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="105">
+      <c r="E4" s="106">
         <f>C4*D4</f>
         <v/>
       </c>
     </row>
-    <row r="5" ht="13.8" customHeight="1" s="2">
+    <row r="5" ht="13.95" customHeight="1" s="2">
       <c r="A5" s="20" t="inlineStr">
         <is>
           <t>Injectable</t>
@@ -5327,18 +5348,18 @@
       <c r="B5" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="105" t="n">
+      <c r="C5" s="106" t="n">
         <v>0.18</v>
       </c>
-      <c r="D5" s="105" t="n">
+      <c r="D5" s="106" t="n">
         <v>0.7</v>
       </c>
-      <c r="E5" s="105">
+      <c r="E5" s="106">
         <f>C5*D5</f>
         <v/>
       </c>
     </row>
-    <row r="6" ht="13.8" customHeight="1" s="2">
+    <row r="6" ht="13.95" customHeight="1" s="2">
       <c r="A6" s="20" t="inlineStr">
         <is>
           <t>Implant</t>
@@ -5347,18 +5368,18 @@
       <c r="B6" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="105" t="n">
+      <c r="C6" s="106" t="n">
         <v>0.02</v>
       </c>
-      <c r="D6" s="105" t="n">
+      <c r="D6" s="106" t="n">
         <v>0.7</v>
       </c>
-      <c r="E6" s="105">
+      <c r="E6" s="106">
         <f>C6*D6</f>
         <v/>
       </c>
     </row>
-    <row r="7" ht="13.8" customHeight="1" s="2">
+    <row r="7" ht="13.95" customHeight="1" s="2">
       <c r="A7" s="20" t="inlineStr">
         <is>
           <t>Pill</t>
@@ -5367,18 +5388,18 @@
       <c r="B7" s="20" t="n">
         <v>0.93</v>
       </c>
-      <c r="C7" s="105" t="n">
+      <c r="C7" s="106" t="n">
         <v>0.45</v>
       </c>
-      <c r="D7" s="105" t="n">
+      <c r="D7" s="106" t="n">
         <v>0.9</v>
       </c>
-      <c r="E7" s="105">
+      <c r="E7" s="106">
         <f>C7*D7</f>
         <v/>
       </c>
     </row>
-    <row r="8" ht="13.8" customHeight="1" s="2">
+    <row r="8" ht="13.95" customHeight="1" s="2">
       <c r="A8" s="20" t="inlineStr">
         <is>
           <t>Withdrawal</t>
@@ -5387,18 +5408,18 @@
       <c r="B8" s="20" t="n">
         <v>0.5</v>
       </c>
-      <c r="C8" s="105" t="n">
+      <c r="C8" s="106" t="n">
         <v>0.03</v>
       </c>
-      <c r="D8" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="105">
+      <c r="D8" s="106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="106">
         <f>C8*D8</f>
         <v/>
       </c>
     </row>
-    <row r="9" ht="13.8" customHeight="1" s="2">
+    <row r="9" ht="13.95" customHeight="1" s="2">
       <c r="A9" s="20" t="inlineStr">
         <is>
           <t>Fertility awareness</t>
@@ -5407,18 +5428,18 @@
       <c r="B9" s="20" t="n">
         <v>0.5</v>
       </c>
-      <c r="C9" s="105" t="n">
+      <c r="C9" s="106" t="n">
         <v>0.11</v>
       </c>
-      <c r="D9" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="105">
+      <c r="D9" s="106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="106">
         <f>C9*D9</f>
         <v/>
       </c>
     </row>
-    <row r="10" ht="13.8" customHeight="1" s="2">
+    <row r="10" ht="13.95" customHeight="1" s="2">
       <c r="A10" s="20" t="inlineStr">
         <is>
           <t>IUD</t>
@@ -5427,13 +5448,13 @@
       <c r="B10" s="20" t="n">
         <v>0.98</v>
       </c>
-      <c r="C10" s="105" t="n">
+      <c r="C10" s="106" t="n">
         <v>0.01</v>
       </c>
-      <c r="D10" s="105" t="n">
+      <c r="D10" s="106" t="n">
         <v>0.6</v>
       </c>
-      <c r="E10" s="105">
+      <c r="E10" s="106">
         <f>C10*D10</f>
         <v/>
       </c>
@@ -5460,7 +5481,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="22.21875" bestFit="1" customWidth="1" style="56" min="1" max="1"/>
+    <col width="22.33203125" bestFit="1" customWidth="1" style="56" min="1" max="1"/>
     <col width="58.88671875" bestFit="1" customWidth="1" style="56" min="2" max="2"/>
     <col width="9.44140625" bestFit="1" customWidth="1" style="56" min="3" max="3"/>
     <col width="11.109375" bestFit="1" customWidth="1" style="56" min="4" max="4"/>
@@ -6650,7 +6671,7 @@
       <c r="N26" s="84" t="n"/>
       <c r="O26" s="84" t="n"/>
     </row>
-    <row r="27" ht="16.05" customHeight="1" s="2">
+    <row r="27" ht="16.2" customHeight="1" s="2">
       <c r="A27" s="57" t="inlineStr">
         <is>
           <t>Non-pregnant WRA</t>
@@ -7383,23 +7404,23 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="58.88671875" bestFit="1" customWidth="1" style="105" min="1" max="1"/>
-    <col width="8.6640625" bestFit="1" customWidth="1" style="105" min="2" max="2"/>
-    <col width="8.88671875" bestFit="1" customWidth="1" style="105" min="3" max="3"/>
-    <col width="18.33203125" bestFit="1" customWidth="1" style="105" min="4" max="4"/>
-    <col width="17.44140625" bestFit="1" customWidth="1" style="105" min="5" max="5"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" style="105" min="6" max="6"/>
-    <col width="9.77734375" bestFit="1" customWidth="1" style="105" min="7" max="7"/>
-    <col width="8.88671875" bestFit="1" customWidth="1" style="105" min="8" max="8"/>
-    <col width="14.77734375" bestFit="1" customWidth="1" style="105" min="9" max="9"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" style="105" min="10" max="10"/>
-    <col width="12.77734375" customWidth="1" style="105" min="11" max="15"/>
-    <col width="12.77734375" customWidth="1" style="105" min="16" max="16384"/>
+    <col width="58.88671875" bestFit="1" customWidth="1" style="106" min="1" max="1"/>
+    <col width="8.6640625" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="8.88671875" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="18.33203125" bestFit="1" customWidth="1" style="106" min="4" max="4"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="8.88671875" bestFit="1" customWidth="1" style="106" min="8" max="8"/>
+    <col width="14.6640625" bestFit="1" customWidth="1" style="106" min="9" max="9"/>
+    <col width="15.33203125" bestFit="1" customWidth="1" style="106" min="10" max="10"/>
+    <col width="12.6640625" customWidth="1" style="106" min="11" max="15"/>
+    <col width="12.6640625" customWidth="1" style="106" min="16" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7408,52 +7429,52 @@
           <t>Program</t>
         </is>
       </c>
-      <c r="B1" s="105" t="inlineStr">
+      <c r="B1" s="106" t="inlineStr">
         <is>
           <t>Stunting</t>
         </is>
       </c>
-      <c r="C1" s="105" t="inlineStr">
+      <c r="C1" s="106" t="inlineStr">
         <is>
           <t>Anaemia</t>
         </is>
       </c>
-      <c r="D1" s="105" t="inlineStr">
+      <c r="D1" s="106" t="inlineStr">
         <is>
           <t>Wasting prevention</t>
         </is>
       </c>
-      <c r="E1" s="105" t="inlineStr">
+      <c r="E1" s="106" t="inlineStr">
         <is>
           <t>Wasting treatment</t>
         </is>
       </c>
-      <c r="F1" s="105" t="inlineStr">
+      <c r="F1" s="106" t="inlineStr">
         <is>
           <t>Breastfeeding</t>
         </is>
       </c>
-      <c r="G1" s="105" t="inlineStr">
+      <c r="G1" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
       </c>
-      <c r="H1" s="105" t="inlineStr">
+      <c r="H1" s="106" t="inlineStr">
         <is>
           <t>Mortality</t>
         </is>
       </c>
-      <c r="I1" s="105" t="inlineStr">
+      <c r="I1" s="106" t="inlineStr">
         <is>
           <t>Birth outcomes</t>
         </is>
       </c>
-      <c r="J1" s="105" t="inlineStr">
+      <c r="J1" s="106" t="inlineStr">
         <is>
           <t>Birth spacing</t>
         </is>
       </c>
-      <c r="K1" s="105" t="inlineStr">
+      <c r="K1" s="106" t="inlineStr">
         <is>
           <t>Birth number</t>
         </is>
@@ -8383,20 +8404,20 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="16.88671875" bestFit="1" customWidth="1" style="105" min="1" max="1"/>
-    <col width="8.6640625" bestFit="1" customWidth="1" style="105" min="2" max="2"/>
-    <col width="8.88671875" bestFit="1" customWidth="1" style="105" min="3" max="3"/>
-    <col width="18.33203125" bestFit="1" customWidth="1" style="105" min="4" max="4"/>
-    <col width="17.44140625" bestFit="1" customWidth="1" style="105" min="5" max="5"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" style="105" min="6" max="6"/>
-    <col width="9.77734375" bestFit="1" customWidth="1" style="105" min="7" max="7"/>
-    <col width="8.88671875" bestFit="1" customWidth="1" style="105" min="8" max="8"/>
-    <col width="14.77734375" bestFit="1" customWidth="1" style="105" min="9" max="9"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" style="105" min="10" max="10"/>
-    <col width="12.77734375" customWidth="1" style="105" min="11" max="15"/>
-    <col width="12.77734375" customWidth="1" style="105" min="16" max="16384"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="106" min="1" max="1"/>
+    <col width="8.6640625" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="8.88671875" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="18.33203125" bestFit="1" customWidth="1" style="106" min="4" max="4"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="8.88671875" bestFit="1" customWidth="1" style="106" min="8" max="8"/>
+    <col width="14.6640625" bestFit="1" customWidth="1" style="106" min="9" max="9"/>
+    <col width="15.33203125" bestFit="1" customWidth="1" style="106" min="10" max="10"/>
+    <col width="12.6640625" customWidth="1" style="106" min="11" max="15"/>
+    <col width="12.6640625" customWidth="1" style="106" min="16" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8405,59 +8426,59 @@
           <t>Age group</t>
         </is>
       </c>
-      <c r="B1" s="105" t="inlineStr">
+      <c r="B1" s="106" t="inlineStr">
         <is>
           <t>Stunting</t>
         </is>
       </c>
-      <c r="C1" s="105" t="inlineStr">
+      <c r="C1" s="106" t="inlineStr">
         <is>
           <t>Anaemia</t>
         </is>
       </c>
-      <c r="D1" s="105" t="inlineStr">
+      <c r="D1" s="106" t="inlineStr">
         <is>
           <t>Wasting prevention</t>
         </is>
       </c>
-      <c r="E1" s="105" t="inlineStr">
+      <c r="E1" s="106" t="inlineStr">
         <is>
           <t>Wasting treatment</t>
         </is>
       </c>
-      <c r="F1" s="105" t="inlineStr">
+      <c r="F1" s="106" t="inlineStr">
         <is>
           <t>Breastfeeding</t>
         </is>
       </c>
-      <c r="G1" s="105" t="inlineStr">
+      <c r="G1" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
       </c>
-      <c r="H1" s="105" t="inlineStr">
+      <c r="H1" s="106" t="inlineStr">
         <is>
           <t>Mortality</t>
         </is>
       </c>
-      <c r="I1" s="105" t="inlineStr">
+      <c r="I1" s="106" t="inlineStr">
         <is>
           <t>Birth outcomes</t>
         </is>
       </c>
-      <c r="J1" s="105" t="inlineStr">
+      <c r="J1" s="106" t="inlineStr">
         <is>
           <t>Birth spacing</t>
         </is>
       </c>
-      <c r="K1" s="105" t="inlineStr">
+      <c r="K1" s="106" t="inlineStr">
         <is>
           <t>Birth number</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="105" t="inlineStr">
+      <c r="A2" s="106" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
@@ -8502,7 +8523,7 @@
       <c r="K2" s="87" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="105" t="inlineStr">
+      <c r="A3" s="106" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
@@ -8547,7 +8568,7 @@
       <c r="K3" s="87" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="105" t="inlineStr">
+      <c r="A4" s="106" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
@@ -8592,7 +8613,7 @@
       <c r="K4" s="87" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="105" t="inlineStr">
+      <c r="A5" s="106" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
@@ -8637,7 +8658,7 @@
       <c r="K5" s="87" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="105" t="inlineStr">
+      <c r="A6" s="106" t="inlineStr">
         <is>
           <t>24-59 months</t>
         </is>
@@ -8682,7 +8703,7 @@
       <c r="K6" s="87" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="105" t="inlineStr">
+      <c r="A7" s="106" t="inlineStr">
         <is>
           <t>PW: 15-19 years</t>
         </is>
@@ -8711,7 +8732,7 @@
       <c r="K7" s="87" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="105" t="inlineStr">
+      <c r="A8" s="106" t="inlineStr">
         <is>
           <t>PW: 20-29 years</t>
         </is>
@@ -8740,7 +8761,7 @@
       <c r="K8" s="87" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="105" t="inlineStr">
+      <c r="A9" s="106" t="inlineStr">
         <is>
           <t>PW: 30-39 years</t>
         </is>
@@ -8769,7 +8790,7 @@
       <c r="K9" s="87" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="105" t="inlineStr">
+      <c r="A10" s="106" t="inlineStr">
         <is>
           <t>PW: 40-49 years</t>
         </is>
@@ -8798,7 +8819,7 @@
       <c r="K10" s="87" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="105" t="inlineStr">
+      <c r="A11" s="106" t="inlineStr">
         <is>
           <t>WRA: 15-19 years</t>
         </is>
@@ -8827,7 +8848,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="105" t="inlineStr">
+      <c r="A12" s="106" t="inlineStr">
         <is>
           <t>WRA: 20-29 years</t>
         </is>
@@ -8852,7 +8873,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="105" t="inlineStr">
+      <c r="A13" s="106" t="inlineStr">
         <is>
           <t>WRA: 30-39 years</t>
         </is>
@@ -8877,7 +8898,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="105" t="inlineStr">
+      <c r="A14" s="106" t="inlineStr">
         <is>
           <t>WRA: 40-49 years</t>
         </is>
@@ -8917,15 +8938,15 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="8.44140625" customWidth="1" style="105" min="1" max="1"/>
-    <col width="16.88671875" customWidth="1" style="105" min="2" max="9"/>
-    <col width="14.44140625" customWidth="1" style="105" min="10" max="14"/>
-    <col width="14.44140625" customWidth="1" style="105" min="15" max="16384"/>
+    <col width="8.44140625" customWidth="1" style="106" min="1" max="1"/>
+    <col width="16.88671875" customWidth="1" style="106" min="2" max="9"/>
+    <col width="14.44140625" customWidth="1" style="106" min="10" max="14"/>
+    <col width="14.44140625" customWidth="1" style="106" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customFormat="1" customHeight="1" s="9">
@@ -9376,21 +9397,11 @@
         <f>IF($A$2+ROW(A14)-2&lt;=end_year,A13+1,"")</f>
         <v/>
       </c>
-      <c r="B14" s="40" t="n">
-        <v>2690000</v>
-      </c>
-      <c r="C14" s="41" t="n">
-        <v>4430738</v>
-      </c>
-      <c r="D14" s="41" t="n">
-        <v>7008703</v>
-      </c>
-      <c r="E14" s="41" t="n">
-        <v>4856898</v>
-      </c>
-      <c r="F14" s="41" t="n">
-        <v>3479917</v>
-      </c>
+      <c r="B14" s="40" t="n"/>
+      <c r="C14" s="41" t="n"/>
+      <c r="D14" s="41" t="n"/>
+      <c r="E14" s="41" t="n"/>
+      <c r="F14" s="41" t="n"/>
       <c r="G14" s="10">
         <f>C14+D14+E14+F14</f>
         <v/>
@@ -9409,21 +9420,11 @@
         <f>IF($A$2+ROW(A15)-2&lt;=end_year,A14+1,"")</f>
         <v/>
       </c>
-      <c r="B15" s="40" t="n">
-        <v>2740000</v>
-      </c>
-      <c r="C15" s="41" t="n">
-        <v>4546624</v>
-      </c>
-      <c r="D15" s="41" t="n">
-        <v>7239465</v>
-      </c>
-      <c r="E15" s="41" t="n">
-        <v>5005361</v>
-      </c>
-      <c r="F15" s="41" t="n">
-        <v>3595278</v>
-      </c>
+      <c r="B15" s="40" t="n"/>
+      <c r="C15" s="41" t="n"/>
+      <c r="D15" s="41" t="n"/>
+      <c r="E15" s="41" t="n"/>
+      <c r="F15" s="41" t="n"/>
       <c r="G15" s="10">
         <f>C15+D15+E15+F15</f>
         <v/>
@@ -10012,6 +10013,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="3E2LSdbO5cWYOfkxLxswaA==" formatRows="1" sort="1" spinCount="100000" hashValue="jm4fOELhKnVZ41a4Zm1quh8zO6dVMK+J36WAlTlifTRD6Nhhzwm0V/yeHz/qcvjqySZtm47YB9fkSA8iSL6ytA=="/>
   <conditionalFormatting sqref="B2:I16 B18:I40 B17:C17 E17:I17">
     <cfRule type="expression" priority="9" dxfId="0">
       <formula>$A2=""</formula>
@@ -10032,16 +10034,16 @@
   <dimension ref="A1:J157"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="48.109375" customWidth="1" style="105" min="1" max="1"/>
-    <col width="15" customWidth="1" style="105" min="2" max="2"/>
-    <col width="14.6640625" customWidth="1" style="105" min="3" max="3"/>
-    <col width="12.77734375" customWidth="1" style="105" min="4" max="8"/>
-    <col width="12.77734375" customWidth="1" style="105" min="9" max="16384"/>
+    <col width="48.109375" customWidth="1" style="106" min="1" max="1"/>
+    <col width="15" customWidth="1" style="106" min="2" max="2"/>
+    <col width="14.6640625" customWidth="1" style="106" min="3" max="3"/>
+    <col width="12.6640625" customWidth="1" style="106" min="4" max="8"/>
+    <col width="12.6640625" customWidth="1" style="106" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10092,12 +10094,12 @@
           <t>Odds ratio for correct breastfeeding</t>
         </is>
       </c>
-      <c r="B2" s="104" t="inlineStr">
+      <c r="B2" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C2" s="105" t="inlineStr">
+      <c r="C2" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10119,7 +10121,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="105" t="inlineStr">
+      <c r="C3" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10142,7 +10144,7 @@
       <c r="J3" s="58" t="n"/>
     </row>
     <row r="4">
-      <c r="C4" s="105" t="inlineStr">
+      <c r="C4" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10165,12 +10167,12 @@
       <c r="J4" s="58" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="104" t="inlineStr">
+      <c r="B5" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C5" s="105" t="inlineStr">
+      <c r="C5" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10193,7 +10195,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="105" t="inlineStr">
+      <c r="C6" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10215,7 +10217,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="C7" s="105" t="inlineStr">
+      <c r="C7" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10237,12 +10239,12 @@
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="104" t="inlineStr">
+      <c r="B8" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C8" s="105" t="inlineStr">
+      <c r="C8" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10264,7 +10266,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="105" t="inlineStr">
+      <c r="C9" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10286,7 +10288,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="105" t="inlineStr">
+      <c r="C10" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10308,12 +10310,12 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="104" t="inlineStr">
+      <c r="B11" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C11" s="105" t="inlineStr">
+      <c r="C11" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10335,7 +10337,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="C12" s="105" t="inlineStr">
+      <c r="C12" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10357,7 +10359,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="105" t="inlineStr">
+      <c r="C13" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10379,12 +10381,12 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="104" t="inlineStr">
+      <c r="B14" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C14" s="105" t="inlineStr">
+      <c r="C14" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10406,7 +10408,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="105" t="inlineStr">
+      <c r="C15" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10428,7 +10430,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="105" t="inlineStr">
+      <c r="C16" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10450,12 +10452,12 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="104" t="inlineStr">
+      <c r="B17" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C17" s="105" t="inlineStr">
+      <c r="C17" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10489,12 +10491,12 @@
           <t>Odds ratio for stunting</t>
         </is>
       </c>
-      <c r="B19" s="104" t="inlineStr">
+      <c r="B19" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C19" s="105" t="inlineStr">
+      <c r="C19" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10516,7 +10518,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="105" t="inlineStr">
+      <c r="C20" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10538,7 +10540,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="105" t="inlineStr">
+      <c r="C21" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10560,12 +10562,12 @@
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="104" t="inlineStr">
+      <c r="B22" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C22" s="105" t="inlineStr">
+      <c r="C22" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10587,7 +10589,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="105" t="inlineStr">
+      <c r="C23" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10609,7 +10611,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="105" t="inlineStr">
+      <c r="C24" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10631,12 +10633,12 @@
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="104" t="inlineStr">
+      <c r="B25" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C25" s="105" t="inlineStr">
+      <c r="C25" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10658,7 +10660,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="105" t="inlineStr">
+      <c r="C26" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10680,7 +10682,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="105" t="inlineStr">
+      <c r="C27" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10702,12 +10704,12 @@
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="104" t="inlineStr">
+      <c r="B28" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C28" s="105" t="inlineStr">
+      <c r="C28" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10729,7 +10731,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="105" t="inlineStr">
+      <c r="C29" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10751,7 +10753,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="105" t="inlineStr">
+      <c r="C30" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10773,12 +10775,12 @@
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="104" t="inlineStr">
+      <c r="B31" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C31" s="105" t="inlineStr">
+      <c r="C31" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10800,7 +10802,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="C32" s="105" t="inlineStr">
+      <c r="C32" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10822,7 +10824,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="105" t="inlineStr">
+      <c r="C33" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10844,12 +10846,12 @@
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="104" t="inlineStr">
+      <c r="B34" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C34" s="105" t="inlineStr">
+      <c r="C34" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10883,12 +10885,12 @@
           <t>Odds ratio for correct complementary feeding</t>
         </is>
       </c>
-      <c r="B36" s="104" t="inlineStr">
+      <c r="B36" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C36" s="105" t="inlineStr">
+      <c r="C36" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10910,7 +10912,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="C37" s="105" t="inlineStr">
+      <c r="C37" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -10932,7 +10934,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="105" t="inlineStr">
+      <c r="C38" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -10954,12 +10956,12 @@
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="104" t="inlineStr">
+      <c r="B39" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C39" s="105" t="inlineStr">
+      <c r="C39" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -10981,7 +10983,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="C40" s="105" t="inlineStr">
+      <c r="C40" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11003,7 +11005,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="C41" s="105" t="inlineStr">
+      <c r="C41" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11025,12 +11027,12 @@
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="104" t="inlineStr">
+      <c r="B42" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C42" s="105" t="inlineStr">
+      <c r="C42" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11052,7 +11054,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="C43" s="105" t="inlineStr">
+      <c r="C43" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11074,7 +11076,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="C44" s="105" t="inlineStr">
+      <c r="C44" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11096,12 +11098,12 @@
       </c>
     </row>
     <row r="45">
-      <c r="B45" s="104" t="inlineStr">
+      <c r="B45" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C45" s="105" t="inlineStr">
+      <c r="C45" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11123,7 +11125,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="C46" s="105" t="inlineStr">
+      <c r="C46" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11145,7 +11147,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="C47" s="105" t="inlineStr">
+      <c r="C47" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11167,12 +11169,12 @@
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="104" t="inlineStr">
+      <c r="B48" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C48" s="105" t="inlineStr">
+      <c r="C48" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11194,7 +11196,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="C49" s="105" t="inlineStr">
+      <c r="C49" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11216,7 +11218,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="C50" s="105" t="inlineStr">
+      <c r="C50" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11238,12 +11240,12 @@
       </c>
     </row>
     <row r="51">
-      <c r="B51" s="104" t="inlineStr">
+      <c r="B51" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C51" s="105" t="inlineStr">
+      <c r="C51" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11326,12 +11328,12 @@
           <t>Odds ratio for correct breastfeeding - lower</t>
         </is>
       </c>
-      <c r="B55" s="104" t="inlineStr">
+      <c r="B55" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C55" s="105" t="inlineStr">
+      <c r="C55" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11358,7 +11360,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="C56" s="105" t="inlineStr">
+      <c r="C56" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11385,7 +11387,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="C57" s="105" t="inlineStr">
+      <c r="C57" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11412,12 +11414,12 @@
       </c>
     </row>
     <row r="58">
-      <c r="B58" s="104" t="inlineStr">
+      <c r="B58" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C58" s="105" t="inlineStr">
+      <c r="C58" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11444,7 +11446,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="C59" s="105" t="inlineStr">
+      <c r="C59" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11471,7 +11473,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="C60" s="105" t="inlineStr">
+      <c r="C60" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11498,12 +11500,12 @@
       </c>
     </row>
     <row r="61">
-      <c r="B61" s="104" t="inlineStr">
+      <c r="B61" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C61" s="105" t="inlineStr">
+      <c r="C61" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11530,7 +11532,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="C62" s="105" t="inlineStr">
+      <c r="C62" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11557,7 +11559,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="C63" s="105" t="inlineStr">
+      <c r="C63" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11584,12 +11586,12 @@
       </c>
     </row>
     <row r="64">
-      <c r="B64" s="104" t="inlineStr">
+      <c r="B64" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C64" s="105" t="inlineStr">
+      <c r="C64" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11616,7 +11618,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="C65" s="105" t="inlineStr">
+      <c r="C65" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11643,7 +11645,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="C66" s="105" t="inlineStr">
+      <c r="C66" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11670,12 +11672,12 @@
       </c>
     </row>
     <row r="67">
-      <c r="B67" s="104" t="inlineStr">
+      <c r="B67" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C67" s="105" t="inlineStr">
+      <c r="C67" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11702,7 +11704,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="C68" s="105" t="inlineStr">
+      <c r="C68" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11729,7 +11731,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="C69" s="105" t="inlineStr">
+      <c r="C69" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11756,12 +11758,12 @@
       </c>
     </row>
     <row r="70">
-      <c r="B70" s="104" t="inlineStr">
+      <c r="B70" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C70" s="105" t="inlineStr">
+      <c r="C70" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11800,12 +11802,12 @@
           <t>Odds ratio for stunting - lower</t>
         </is>
       </c>
-      <c r="B72" s="104" t="inlineStr">
+      <c r="B72" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C72" s="105" t="inlineStr">
+      <c r="C72" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11832,7 +11834,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="C73" s="105" t="inlineStr">
+      <c r="C73" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11859,7 +11861,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="C74" s="105" t="inlineStr">
+      <c r="C74" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11886,12 +11888,12 @@
       </c>
     </row>
     <row r="75">
-      <c r="B75" s="104" t="inlineStr">
+      <c r="B75" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C75" s="105" t="inlineStr">
+      <c r="C75" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -11918,7 +11920,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="C76" s="105" t="inlineStr">
+      <c r="C76" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -11945,7 +11947,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="C77" s="105" t="inlineStr">
+      <c r="C77" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -11972,12 +11974,12 @@
       </c>
     </row>
     <row r="78">
-      <c r="B78" s="104" t="inlineStr">
+      <c r="B78" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C78" s="105" t="inlineStr">
+      <c r="C78" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12004,7 +12006,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="C79" s="105" t="inlineStr">
+      <c r="C79" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12031,7 +12033,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="C80" s="105" t="inlineStr">
+      <c r="C80" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12058,12 +12060,12 @@
       </c>
     </row>
     <row r="81">
-      <c r="B81" s="104" t="inlineStr">
+      <c r="B81" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C81" s="105" t="inlineStr">
+      <c r="C81" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12090,7 +12092,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="C82" s="105" t="inlineStr">
+      <c r="C82" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12117,7 +12119,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="C83" s="105" t="inlineStr">
+      <c r="C83" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12144,12 +12146,12 @@
       </c>
     </row>
     <row r="84">
-      <c r="B84" s="104" t="inlineStr">
+      <c r="B84" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C84" s="105" t="inlineStr">
+      <c r="C84" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12176,7 +12178,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="C85" s="105" t="inlineStr">
+      <c r="C85" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12203,7 +12205,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="C86" s="105" t="inlineStr">
+      <c r="C86" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12230,12 +12232,12 @@
       </c>
     </row>
     <row r="87">
-      <c r="B87" s="104" t="inlineStr">
+      <c r="B87" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C87" s="105" t="inlineStr">
+      <c r="C87" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12274,12 +12276,12 @@
           <t>Odds ratio for correct complementary feeding - lower</t>
         </is>
       </c>
-      <c r="B89" s="104" t="inlineStr">
+      <c r="B89" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C89" s="105" t="inlineStr">
+      <c r="C89" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12306,7 +12308,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="C90" s="105" t="inlineStr">
+      <c r="C90" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12333,7 +12335,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="C91" s="105" t="inlineStr">
+      <c r="C91" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12360,12 +12362,12 @@
       </c>
     </row>
     <row r="92">
-      <c r="B92" s="104" t="inlineStr">
+      <c r="B92" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C92" s="105" t="inlineStr">
+      <c r="C92" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12392,7 +12394,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="C93" s="105" t="inlineStr">
+      <c r="C93" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12419,7 +12421,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="C94" s="105" t="inlineStr">
+      <c r="C94" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12446,12 +12448,12 @@
       </c>
     </row>
     <row r="95">
-      <c r="B95" s="104" t="inlineStr">
+      <c r="B95" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C95" s="105" t="inlineStr">
+      <c r="C95" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12478,7 +12480,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="C96" s="105" t="inlineStr">
+      <c r="C96" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12505,7 +12507,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="C97" s="105" t="inlineStr">
+      <c r="C97" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12532,12 +12534,12 @@
       </c>
     </row>
     <row r="98">
-      <c r="B98" s="104" t="inlineStr">
+      <c r="B98" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C98" s="105" t="inlineStr">
+      <c r="C98" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12564,7 +12566,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="C99" s="105" t="inlineStr">
+      <c r="C99" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12591,7 +12593,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="C100" s="105" t="inlineStr">
+      <c r="C100" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12618,12 +12620,12 @@
       </c>
     </row>
     <row r="101">
-      <c r="B101" s="104" t="inlineStr">
+      <c r="B101" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C101" s="105" t="inlineStr">
+      <c r="C101" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12650,7 +12652,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="C102" s="105" t="inlineStr">
+      <c r="C102" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12677,7 +12679,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="C103" s="105" t="inlineStr">
+      <c r="C103" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12704,12 +12706,12 @@
       </c>
     </row>
     <row r="104">
-      <c r="B104" s="104" t="inlineStr">
+      <c r="B104" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C104" s="105" t="inlineStr">
+      <c r="C104" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12797,12 +12799,12 @@
           <t>Odds ratio for correct breastfeeding - upper</t>
         </is>
       </c>
-      <c r="B108" s="104" t="inlineStr">
+      <c r="B108" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C108" s="105" t="inlineStr">
+      <c r="C108" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12829,7 +12831,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="C109" s="105" t="inlineStr">
+      <c r="C109" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12856,7 +12858,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="C110" s="105" t="inlineStr">
+      <c r="C110" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12883,12 +12885,12 @@
       </c>
     </row>
     <row r="111">
-      <c r="B111" s="104" t="inlineStr">
+      <c r="B111" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C111" s="105" t="inlineStr">
+      <c r="C111" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -12915,7 +12917,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="C112" s="105" t="inlineStr">
+      <c r="C112" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -12942,7 +12944,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="C113" s="105" t="inlineStr">
+      <c r="C113" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -12969,12 +12971,12 @@
       </c>
     </row>
     <row r="114">
-      <c r="B114" s="104" t="inlineStr">
+      <c r="B114" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C114" s="105" t="inlineStr">
+      <c r="C114" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13001,7 +13003,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="C115" s="105" t="inlineStr">
+      <c r="C115" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13028,7 +13030,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="C116" s="105" t="inlineStr">
+      <c r="C116" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13055,12 +13057,12 @@
       </c>
     </row>
     <row r="117">
-      <c r="B117" s="104" t="inlineStr">
+      <c r="B117" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C117" s="105" t="inlineStr">
+      <c r="C117" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13087,7 +13089,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="C118" s="105" t="inlineStr">
+      <c r="C118" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13114,7 +13116,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="C119" s="105" t="inlineStr">
+      <c r="C119" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13141,12 +13143,12 @@
       </c>
     </row>
     <row r="120">
-      <c r="B120" s="104" t="inlineStr">
+      <c r="B120" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C120" s="105" t="inlineStr">
+      <c r="C120" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13173,7 +13175,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="C121" s="105" t="inlineStr">
+      <c r="C121" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13200,7 +13202,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="C122" s="105" t="inlineStr">
+      <c r="C122" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13227,12 +13229,12 @@
       </c>
     </row>
     <row r="123">
-      <c r="B123" s="104" t="inlineStr">
+      <c r="B123" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C123" s="105" t="inlineStr">
+      <c r="C123" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13271,12 +13273,12 @@
           <t>Odds ratio for stunting - upper</t>
         </is>
       </c>
-      <c r="B125" s="104" t="inlineStr">
+      <c r="B125" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C125" s="105" t="inlineStr">
+      <c r="C125" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13303,7 +13305,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="C126" s="105" t="inlineStr">
+      <c r="C126" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13330,7 +13332,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="C127" s="105" t="inlineStr">
+      <c r="C127" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13357,12 +13359,12 @@
       </c>
     </row>
     <row r="128">
-      <c r="B128" s="104" t="inlineStr">
+      <c r="B128" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C128" s="105" t="inlineStr">
+      <c r="C128" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13389,7 +13391,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="C129" s="105" t="inlineStr">
+      <c r="C129" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13416,7 +13418,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="C130" s="105" t="inlineStr">
+      <c r="C130" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13443,12 +13445,12 @@
       </c>
     </row>
     <row r="131">
-      <c r="B131" s="104" t="inlineStr">
+      <c r="B131" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C131" s="105" t="inlineStr">
+      <c r="C131" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13475,7 +13477,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="C132" s="105" t="inlineStr">
+      <c r="C132" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13502,7 +13504,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="C133" s="105" t="inlineStr">
+      <c r="C133" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13529,12 +13531,12 @@
       </c>
     </row>
     <row r="134">
-      <c r="B134" s="104" t="inlineStr">
+      <c r="B134" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C134" s="105" t="inlineStr">
+      <c r="C134" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13561,7 +13563,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="C135" s="105" t="inlineStr">
+      <c r="C135" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13588,7 +13590,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="C136" s="105" t="inlineStr">
+      <c r="C136" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13615,12 +13617,12 @@
       </c>
     </row>
     <row r="137">
-      <c r="B137" s="104" t="inlineStr">
+      <c r="B137" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C137" s="105" t="inlineStr">
+      <c r="C137" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13647,7 +13649,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="C138" s="105" t="inlineStr">
+      <c r="C138" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13674,7 +13676,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="C139" s="105" t="inlineStr">
+      <c r="C139" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13701,12 +13703,12 @@
       </c>
     </row>
     <row r="140">
-      <c r="B140" s="104" t="inlineStr">
+      <c r="B140" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C140" s="105" t="inlineStr">
+      <c r="C140" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13745,12 +13747,12 @@
           <t>Odds ratio for correct complementary feeding - upper</t>
         </is>
       </c>
-      <c r="B142" s="104" t="inlineStr">
+      <c r="B142" s="105" t="inlineStr">
         <is>
           <t>Pregnant women</t>
         </is>
       </c>
-      <c r="C142" s="105" t="inlineStr">
+      <c r="C142" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13777,7 +13779,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="C143" s="105" t="inlineStr">
+      <c r="C143" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13804,7 +13806,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="C144" s="105" t="inlineStr">
+      <c r="C144" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13831,12 +13833,12 @@
       </c>
     </row>
     <row r="145">
-      <c r="B145" s="104" t="inlineStr">
+      <c r="B145" s="105" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C145" s="105" t="inlineStr">
+      <c r="C145" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13863,7 +13865,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="C146" s="105" t="inlineStr">
+      <c r="C146" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13890,7 +13892,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="C147" s="105" t="inlineStr">
+      <c r="C147" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -13917,12 +13919,12 @@
       </c>
     </row>
     <row r="148">
-      <c r="B148" s="104" t="inlineStr">
+      <c r="B148" s="105" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C148" s="105" t="inlineStr">
+      <c r="C148" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -13949,7 +13951,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="C149" s="105" t="inlineStr">
+      <c r="C149" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -13976,7 +13978,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="C150" s="105" t="inlineStr">
+      <c r="C150" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -14003,12 +14005,12 @@
       </c>
     </row>
     <row r="151">
-      <c r="B151" s="104" t="inlineStr">
+      <c r="B151" s="105" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C151" s="105" t="inlineStr">
+      <c r="C151" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -14035,7 +14037,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="C152" s="105" t="inlineStr">
+      <c r="C152" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -14062,7 +14064,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="C153" s="105" t="inlineStr">
+      <c r="C153" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -14089,12 +14091,12 @@
       </c>
     </row>
     <row r="154">
-      <c r="B154" s="104" t="inlineStr">
+      <c r="B154" s="105" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C154" s="105" t="inlineStr">
+      <c r="C154" s="106" t="inlineStr">
         <is>
           <t>Health facility</t>
         </is>
@@ -14121,7 +14123,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="C155" s="105" t="inlineStr">
+      <c r="C155" s="106" t="inlineStr">
         <is>
           <t>Community</t>
         </is>
@@ -14148,7 +14150,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="C156" s="105" t="inlineStr">
+      <c r="C156" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -14175,12 +14177,12 @@
       </c>
     </row>
     <row r="157">
-      <c r="B157" s="104" t="inlineStr">
+      <c r="B157" s="105" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C157" s="105" t="inlineStr">
+      <c r="C157" s="106" t="inlineStr">
         <is>
           <t>Mass media</t>
         </is>
@@ -14208,6 +14210,42 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -14217,42 +14255,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
@@ -14269,18 +14271,18 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="23.88671875" customWidth="1" style="105" min="1" max="1"/>
-    <col width="34.109375" customWidth="1" style="105" min="2" max="2"/>
-    <col width="11.33203125" bestFit="1" customWidth="1" style="105" min="3" max="3"/>
-    <col width="11.88671875" customWidth="1" style="105" min="4" max="4"/>
-    <col width="15" customWidth="1" style="105" min="5" max="6"/>
-    <col width="16.109375" customWidth="1" style="105" min="7" max="11"/>
-    <col width="16.109375" customWidth="1" style="105" min="12" max="16384"/>
+    <col width="23.88671875" customWidth="1" style="106" min="1" max="1"/>
+    <col width="34.109375" customWidth="1" style="106" min="2" max="2"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="11.88671875" customWidth="1" style="106" min="4" max="4"/>
+    <col width="15" customWidth="1" style="106" min="5" max="6"/>
+    <col width="16.109375" customWidth="1" style="106" min="7" max="11"/>
+    <col width="16.109375" customWidth="1" style="106" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customFormat="1" customHeight="1" s="69">
@@ -15644,19 +15646,19 @@
   <dimension ref="A1:P328"/>
   <sheetViews>
     <sheetView topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I328" sqref="I328"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="27.21875" customWidth="1" style="105" min="1" max="1"/>
-    <col width="26.88671875" customWidth="1" style="105" min="2" max="2"/>
-    <col width="18.33203125" customWidth="1" style="105" min="3" max="3"/>
-    <col width="14.77734375" customWidth="1" style="105" min="4" max="8"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" style="105" min="9" max="12"/>
-    <col width="16.88671875" bestFit="1" customWidth="1" style="105" min="13" max="16"/>
-    <col width="12.77734375" customWidth="1" style="105" min="17" max="21"/>
-    <col width="12.77734375" customWidth="1" style="105" min="22" max="16384"/>
+    <col width="27.33203125" customWidth="1" style="106" min="1" max="1"/>
+    <col width="26.88671875" customWidth="1" style="106" min="2" max="2"/>
+    <col width="18.33203125" customWidth="1" style="106" min="3" max="3"/>
+    <col width="14.6640625" customWidth="1" style="106" min="4" max="8"/>
+    <col width="15.33203125" bestFit="1" customWidth="1" style="106" min="9" max="12"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="106" min="13" max="16"/>
+    <col width="12.6640625" customWidth="1" style="106" min="17" max="21"/>
+    <col width="12.6640625" customWidth="1" style="106" min="22" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="69">
@@ -15718,7 +15720,7 @@
     </row>
     <row r="3">
       <c r="A3" s="57" t="n"/>
-      <c r="B3" s="105" t="inlineStr">
+      <c r="B3" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -15843,7 +15845,7 @@
       <c r="P6" s="77" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="105" t="inlineStr">
+      <c r="B7" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -15968,7 +15970,7 @@
       <c r="P10" s="77" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="105" t="inlineStr">
+      <c r="B11" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -16093,7 +16095,7 @@
       <c r="P14" s="77" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="105" t="inlineStr">
+      <c r="B15" s="106" t="inlineStr">
         <is>
           <t>Malaria</t>
         </is>
@@ -16218,7 +16220,7 @@
       <c r="P18" s="77" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="105" t="inlineStr">
+      <c r="B19" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -16343,7 +16345,7 @@
       <c r="P22" s="77" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="105" t="inlineStr">
+      <c r="B23" s="106" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
@@ -16526,7 +16528,7 @@
     </row>
     <row r="30">
       <c r="A30" s="57" t="n"/>
-      <c r="B30" s="105" t="inlineStr">
+      <c r="B30" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -16651,7 +16653,7 @@
       <c r="P33" s="77" t="n"/>
     </row>
     <row r="34">
-      <c r="B34" s="105" t="inlineStr">
+      <c r="B34" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -16776,7 +16778,7 @@
       <c r="P37" s="77" t="n"/>
     </row>
     <row r="38">
-      <c r="B38" s="105" t="inlineStr">
+      <c r="B38" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -16901,7 +16903,7 @@
       <c r="P41" s="77" t="n"/>
     </row>
     <row r="42">
-      <c r="B42" s="105" t="inlineStr">
+      <c r="B42" s="106" t="inlineStr">
         <is>
           <t>Malaria</t>
         </is>
@@ -17026,7 +17028,7 @@
       <c r="P45" s="77" t="n"/>
     </row>
     <row r="46">
-      <c r="B46" s="105" t="inlineStr">
+      <c r="B46" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -17151,7 +17153,7 @@
       <c r="P49" s="77" t="n"/>
     </row>
     <row r="50">
-      <c r="B50" s="105" t="inlineStr">
+      <c r="B50" s="106" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
@@ -17330,7 +17332,7 @@
     </row>
     <row r="57">
       <c r="A57" s="57" t="n"/>
-      <c r="B57" s="105" t="inlineStr">
+      <c r="B57" s="106" t="inlineStr">
         <is>
           <t>Antepartum haemorrhage</t>
         </is>
@@ -17383,7 +17385,7 @@
       <c r="P58" s="77" t="n"/>
     </row>
     <row r="59">
-      <c r="B59" s="105" t="inlineStr">
+      <c r="B59" s="106" t="inlineStr">
         <is>
           <t>Intrapartum haemorrhage</t>
         </is>
@@ -17436,7 +17438,7 @@
       <c r="P60" s="77" t="n"/>
     </row>
     <row r="61">
-      <c r="B61" s="105" t="inlineStr">
+      <c r="B61" s="106" t="inlineStr">
         <is>
           <t>Postpartum haemorrhage</t>
         </is>
@@ -17551,7 +17553,7 @@
     </row>
     <row r="66">
       <c r="A66" s="81" t="n"/>
-      <c r="B66" s="105" t="inlineStr">
+      <c r="B66" s="106" t="inlineStr">
         <is>
           <t>Neonatal diarrhoea</t>
         </is>
@@ -17676,7 +17678,7 @@
       <c r="P69" s="77" t="n"/>
     </row>
     <row r="70">
-      <c r="B70" s="105" t="inlineStr">
+      <c r="B70" s="106" t="inlineStr">
         <is>
           <t>Neonatal sepsis</t>
         </is>
@@ -17801,7 +17803,7 @@
       <c r="P73" s="77" t="n"/>
     </row>
     <row r="74">
-      <c r="B74" s="105" t="inlineStr">
+      <c r="B74" s="106" t="inlineStr">
         <is>
           <t>Neonatal pneumonia</t>
         </is>
@@ -17926,7 +17928,7 @@
       <c r="P77" s="77" t="n"/>
     </row>
     <row r="78">
-      <c r="B78" s="105" t="inlineStr">
+      <c r="B78" s="106" t="inlineStr">
         <is>
           <t>Neonatal prematurity</t>
         </is>
@@ -18051,7 +18053,7 @@
       <c r="P81" s="77" t="n"/>
     </row>
     <row r="82">
-      <c r="B82" s="105" t="inlineStr">
+      <c r="B82" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -18176,7 +18178,7 @@
       <c r="P85" s="77" t="n"/>
     </row>
     <row r="86">
-      <c r="B86" s="105" t="inlineStr">
+      <c r="B86" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -18301,7 +18303,7 @@
       <c r="P89" s="77" t="n"/>
     </row>
     <row r="90">
-      <c r="B90" s="105" t="inlineStr">
+      <c r="B90" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -18426,7 +18428,7 @@
       <c r="P93" s="77" t="n"/>
     </row>
     <row r="94">
-      <c r="B94" s="105" t="inlineStr">
+      <c r="B94" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -18551,7 +18553,7 @@
       <c r="P97" s="77" t="n"/>
     </row>
     <row r="98">
-      <c r="B98" s="105" t="inlineStr">
+      <c r="B98" s="106" t="inlineStr">
         <is>
           <t>Pertussis</t>
         </is>
@@ -18919,7 +18921,7 @@
     </row>
     <row r="113">
       <c r="A113" s="57" t="n"/>
-      <c r="B113" s="105" t="inlineStr">
+      <c r="B113" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -19032,7 +19034,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="B117" s="105" t="inlineStr">
+      <c r="B117" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -19145,7 +19147,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="B121" s="105" t="inlineStr">
+      <c r="B121" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -19258,7 +19260,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="B125" s="105" t="inlineStr">
+      <c r="B125" s="106" t="inlineStr">
         <is>
           <t>Malaria</t>
         </is>
@@ -19371,7 +19373,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="B129" s="105" t="inlineStr">
+      <c r="B129" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -19484,7 +19486,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="B133" s="105" t="inlineStr">
+      <c r="B133" s="106" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
@@ -19654,7 +19656,7 @@
     </row>
     <row r="140">
       <c r="A140" s="57" t="n"/>
-      <c r="B140" s="105" t="inlineStr">
+      <c r="B140" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -19767,7 +19769,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="B144" s="105" t="inlineStr">
+      <c r="B144" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -19880,7 +19882,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="B148" s="105" t="inlineStr">
+      <c r="B148" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -19993,7 +19995,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="B152" s="105" t="inlineStr">
+      <c r="B152" s="106" t="inlineStr">
         <is>
           <t>Malaria</t>
         </is>
@@ -20106,7 +20108,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="B156" s="105" t="inlineStr">
+      <c r="B156" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -20219,7 +20221,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="B160" s="105" t="inlineStr">
+      <c r="B160" s="106" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
@@ -20389,7 +20391,7 @@
     </row>
     <row r="167">
       <c r="A167" s="57" t="n"/>
-      <c r="B167" s="105" t="inlineStr">
+      <c r="B167" s="106" t="inlineStr">
         <is>
           <t>Antepartum haemorrhage</t>
         </is>
@@ -20442,7 +20444,7 @@
       <c r="H168" s="77" t="n"/>
     </row>
     <row r="169">
-      <c r="B169" s="105" t="inlineStr">
+      <c r="B169" s="106" t="inlineStr">
         <is>
           <t>Intrapartum haemorrhage</t>
         </is>
@@ -20495,7 +20497,7 @@
       <c r="H170" s="77" t="n"/>
     </row>
     <row r="171">
-      <c r="B171" s="105" t="inlineStr">
+      <c r="B171" s="106" t="inlineStr">
         <is>
           <t>Postpartum haemorrhage</t>
         </is>
@@ -20609,7 +20611,7 @@
     </row>
     <row r="176">
       <c r="A176" s="81" t="n"/>
-      <c r="B176" s="105" t="inlineStr">
+      <c r="B176" s="106" t="inlineStr">
         <is>
           <t>Neonatal diarrhoea</t>
         </is>
@@ -20718,7 +20720,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="B180" s="105" t="inlineStr">
+      <c r="B180" s="106" t="inlineStr">
         <is>
           <t>Neonatal sepsis</t>
         </is>
@@ -20827,7 +20829,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="B184" s="105" t="inlineStr">
+      <c r="B184" s="106" t="inlineStr">
         <is>
           <t>Neonatal pneumonia</t>
         </is>
@@ -20936,7 +20938,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="B188" s="105" t="inlineStr">
+      <c r="B188" s="106" t="inlineStr">
         <is>
           <t>Neonatal prematurity</t>
         </is>
@@ -21045,7 +21047,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="B192" s="105" t="inlineStr">
+      <c r="B192" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -21154,7 +21156,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="B196" s="105" t="inlineStr">
+      <c r="B196" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -21263,7 +21265,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="B200" s="105" t="inlineStr">
+      <c r="B200" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -21372,7 +21374,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="B204" s="105" t="inlineStr">
+      <c r="B204" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -21481,7 +21483,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="B208" s="105" t="inlineStr">
+      <c r="B208" s="106" t="inlineStr">
         <is>
           <t>Pertussis</t>
         </is>
@@ -21818,7 +21820,7 @@
     </row>
     <row r="223">
       <c r="A223" s="57" t="n"/>
-      <c r="B223" s="105" t="inlineStr">
+      <c r="B223" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -21935,7 +21937,7 @@
       <c r="I226" s="77" t="n"/>
     </row>
     <row r="227">
-      <c r="B227" s="105" t="inlineStr">
+      <c r="B227" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -22052,7 +22054,7 @@
       <c r="I230" s="77" t="n"/>
     </row>
     <row r="231">
-      <c r="B231" s="105" t="inlineStr">
+      <c r="B231" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -22169,7 +22171,7 @@
       <c r="I234" s="77" t="n"/>
     </row>
     <row r="235">
-      <c r="B235" s="105" t="inlineStr">
+      <c r="B235" s="106" t="inlineStr">
         <is>
           <t>Malaria</t>
         </is>
@@ -22286,7 +22288,7 @@
       <c r="I238" s="77" t="n"/>
     </row>
     <row r="239">
-      <c r="B239" s="105" t="inlineStr">
+      <c r="B239" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -22403,7 +22405,7 @@
       <c r="I242" s="77" t="n"/>
     </row>
     <row r="243">
-      <c r="B243" s="105" t="inlineStr">
+      <c r="B243" s="106" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
@@ -22579,7 +22581,7 @@
     </row>
     <row r="250">
       <c r="A250" s="57" t="n"/>
-      <c r="B250" s="105" t="inlineStr">
+      <c r="B250" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -22696,7 +22698,7 @@
       <c r="I253" s="77" t="n"/>
     </row>
     <row r="254">
-      <c r="B254" s="105" t="inlineStr">
+      <c r="B254" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -22813,7 +22815,7 @@
       <c r="I257" s="77" t="n"/>
     </row>
     <row r="258">
-      <c r="B258" s="105" t="inlineStr">
+      <c r="B258" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -22930,7 +22932,7 @@
       <c r="I261" s="77" t="n"/>
     </row>
     <row r="262">
-      <c r="B262" s="105" t="inlineStr">
+      <c r="B262" s="106" t="inlineStr">
         <is>
           <t>Malaria</t>
         </is>
@@ -23047,7 +23049,7 @@
       <c r="I265" s="77" t="n"/>
     </row>
     <row r="266">
-      <c r="B266" s="105" t="inlineStr">
+      <c r="B266" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -23164,7 +23166,7 @@
       <c r="I269" s="77" t="n"/>
     </row>
     <row r="270">
-      <c r="B270" s="105" t="inlineStr">
+      <c r="B270" s="106" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
@@ -23339,7 +23341,7 @@
     </row>
     <row r="277">
       <c r="A277" s="57" t="n"/>
-      <c r="B277" s="105" t="inlineStr">
+      <c r="B277" s="106" t="inlineStr">
         <is>
           <t>Antepartum haemorrhage</t>
         </is>
@@ -23392,7 +23394,7 @@
       <c r="H278" s="77" t="n"/>
     </row>
     <row r="279">
-      <c r="B279" s="105" t="inlineStr">
+      <c r="B279" s="106" t="inlineStr">
         <is>
           <t>Intrapartum haemorrhage</t>
         </is>
@@ -23445,7 +23447,7 @@
       <c r="H280" s="77" t="n"/>
     </row>
     <row r="281">
-      <c r="B281" s="105" t="inlineStr">
+      <c r="B281" s="106" t="inlineStr">
         <is>
           <t>Postpartum haemorrhage</t>
         </is>
@@ -23561,7 +23563,7 @@
     </row>
     <row r="286">
       <c r="A286" s="81" t="n"/>
-      <c r="B286" s="105" t="inlineStr">
+      <c r="B286" s="106" t="inlineStr">
         <is>
           <t>Neonatal diarrhoea</t>
         </is>
@@ -23674,7 +23676,7 @@
       <c r="I289" s="77" t="n"/>
     </row>
     <row r="290">
-      <c r="B290" s="105" t="inlineStr">
+      <c r="B290" s="106" t="inlineStr">
         <is>
           <t>Neonatal sepsis</t>
         </is>
@@ -23787,7 +23789,7 @@
       <c r="I293" s="77" t="n"/>
     </row>
     <row r="294">
-      <c r="B294" s="105" t="inlineStr">
+      <c r="B294" s="106" t="inlineStr">
         <is>
           <t>Neonatal pneumonia</t>
         </is>
@@ -23900,7 +23902,7 @@
       <c r="I297" s="77" t="n"/>
     </row>
     <row r="298">
-      <c r="B298" s="105" t="inlineStr">
+      <c r="B298" s="106" t="inlineStr">
         <is>
           <t>Neonatal prematurity</t>
         </is>
@@ -24013,7 +24015,7 @@
       <c r="I301" s="77" t="n"/>
     </row>
     <row r="302">
-      <c r="B302" s="105" t="inlineStr">
+      <c r="B302" s="106" t="inlineStr">
         <is>
           <t>Diarrhoea</t>
         </is>
@@ -24126,7 +24128,7 @@
       <c r="I305" s="77" t="n"/>
     </row>
     <row r="306">
-      <c r="B306" s="105" t="inlineStr">
+      <c r="B306" s="106" t="inlineStr">
         <is>
           <t>Pneumonia</t>
         </is>
@@ -24239,7 +24241,7 @@
       <c r="I309" s="77" t="n"/>
     </row>
     <row r="310">
-      <c r="B310" s="105" t="inlineStr">
+      <c r="B310" s="106" t="inlineStr">
         <is>
           <t>Measles</t>
         </is>
@@ -24352,7 +24354,7 @@
       <c r="I313" s="77" t="n"/>
     </row>
     <row r="314">
-      <c r="B314" s="105" t="inlineStr">
+      <c r="B314" s="106" t="inlineStr">
         <is>
           <t>Meningitis</t>
         </is>
@@ -24465,7 +24467,7 @@
       <c r="I317" s="77" t="n"/>
     </row>
     <row r="318">
-      <c r="B318" s="105" t="inlineStr">
+      <c r="B318" s="106" t="inlineStr">
         <is>
           <t>Pertussis</t>
         </is>
@@ -24760,20 +24762,20 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="44.88671875" customWidth="1" style="105" min="1" max="1"/>
-    <col width="44.44140625" customWidth="1" style="105" min="2" max="2"/>
-    <col width="17.77734375" customWidth="1" style="105" min="3" max="3"/>
-    <col width="17.5546875" customWidth="1" style="105" min="4" max="4"/>
-    <col width="17.21875" customWidth="1" style="105" min="5" max="5"/>
-    <col width="15" customWidth="1" style="105" min="6" max="6"/>
-    <col width="13.6640625" customWidth="1" style="105" min="7" max="7"/>
-    <col width="12.77734375" customWidth="1" style="105" min="8" max="12"/>
-    <col width="12.77734375" customWidth="1" style="105" min="13" max="16384"/>
+    <col width="44.88671875" customWidth="1" style="106" min="1" max="1"/>
+    <col width="44.44140625" customWidth="1" style="106" min="2" max="2"/>
+    <col width="17.6640625" customWidth="1" style="106" min="3" max="3"/>
+    <col width="17.5546875" customWidth="1" style="106" min="4" max="4"/>
+    <col width="17.33203125" customWidth="1" style="106" min="5" max="5"/>
+    <col width="15" customWidth="1" style="106" min="6" max="6"/>
+    <col width="13.6640625" customWidth="1" style="106" min="7" max="7"/>
+    <col width="12.6640625" customWidth="1" style="106" min="8" max="12"/>
+    <col width="12.6640625" customWidth="1" style="106" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customFormat="1" customHeight="1" s="69">
@@ -26030,16 +26032,16 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="52.21875" customWidth="1" style="105" min="1" max="1"/>
-    <col width="16.109375" customWidth="1" style="105" min="2" max="6"/>
-    <col width="17.21875" customWidth="1" style="105" min="7" max="7"/>
-    <col width="16.109375" customWidth="1" style="105" min="8" max="13"/>
-    <col width="16.109375" customWidth="1" style="105" min="14" max="16384"/>
+    <col width="52.33203125" customWidth="1" style="106" min="1" max="1"/>
+    <col width="16.109375" customWidth="1" style="106" min="2" max="6"/>
+    <col width="17.33203125" customWidth="1" style="106" min="7" max="7"/>
+    <col width="16.109375" customWidth="1" style="106" min="8" max="13"/>
+    <col width="16.109375" customWidth="1" style="106" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="2">
@@ -27044,16 +27046,16 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="22.5546875" customWidth="1" style="105" min="1" max="1"/>
-    <col width="58.88671875" bestFit="1" customWidth="1" style="105" min="2" max="2"/>
-    <col width="15" customWidth="1" style="105" min="3" max="15"/>
-    <col width="12.77734375" customWidth="1" style="105" min="16" max="20"/>
-    <col width="12.77734375" customWidth="1" style="105" min="21" max="16384"/>
+    <col width="22.5546875" customWidth="1" style="106" min="1" max="1"/>
+    <col width="58.88671875" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="15" customWidth="1" style="106" min="3" max="15"/>
+    <col width="12.6640625" customWidth="1" style="106" min="16" max="20"/>
+    <col width="12.6640625" customWidth="1" style="106" min="21" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="35.25" customHeight="1" s="2">
@@ -27592,7 +27594,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" ht="13.05" customHeight="1" s="2">
+    <row r="13" ht="13.2" customHeight="1" s="2">
       <c r="B13" s="70" t="inlineStr">
         <is>
           <t>Micronutrient powders</t>
@@ -30126,16 +30128,16 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="21.33203125" customWidth="1" style="105" min="1" max="1"/>
-    <col width="27.77734375" customWidth="1" style="105" min="2" max="2"/>
-    <col width="15.5546875" customWidth="1" style="105" min="3" max="7"/>
-    <col width="12.77734375" customWidth="1" style="105" min="8" max="12"/>
-    <col width="12.77734375" customWidth="1" style="105" min="13" max="16384"/>
+    <col width="21.33203125" customWidth="1" style="106" min="1" max="1"/>
+    <col width="27.6640625" customWidth="1" style="106" min="2" max="2"/>
+    <col width="15.5546875" customWidth="1" style="106" min="3" max="7"/>
+    <col width="12.6640625" customWidth="1" style="106" min="8" max="12"/>
+    <col width="12.6640625" customWidth="1" style="106" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -30467,21 +30469,21 @@
   <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111:XFD111"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
     <col width="53" customWidth="1" style="74" min="1" max="1"/>
     <col width="30.5546875" customWidth="1" style="74" min="2" max="2"/>
-    <col width="24.77734375" customWidth="1" style="74" min="3" max="3"/>
-    <col width="15" customWidth="1" style="105" min="4" max="4"/>
-    <col width="13.6640625" customWidth="1" style="105" min="5" max="5"/>
-    <col width="14.44140625" customWidth="1" style="105" min="6" max="6"/>
-    <col width="12.77734375" customWidth="1" style="105" min="7" max="7"/>
-    <col width="17.5546875" customWidth="1" style="105" min="8" max="8"/>
-    <col width="12.77734375" customWidth="1" style="105" min="9" max="13"/>
-    <col width="12.77734375" customWidth="1" style="105" min="14" max="16384"/>
+    <col width="24.6640625" customWidth="1" style="74" min="3" max="3"/>
+    <col width="15" customWidth="1" style="106" min="4" max="4"/>
+    <col width="13.6640625" customWidth="1" style="106" min="5" max="5"/>
+    <col width="14.44140625" customWidth="1" style="106" min="6" max="6"/>
+    <col width="12.6640625" customWidth="1" style="106" min="7" max="7"/>
+    <col width="17.5546875" customWidth="1" style="106" min="8" max="8"/>
+    <col width="12.6640625" customWidth="1" style="106" min="9" max="13"/>
+    <col width="12.6640625" customWidth="1" style="106" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -35181,17 +35183,17 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="28" customWidth="1" style="105" min="1" max="1"/>
-    <col width="27.44140625" customWidth="1" style="105" min="2" max="2"/>
-    <col width="23.6640625" customWidth="1" style="105" min="3" max="3"/>
-    <col width="17.21875" customWidth="1" style="105" min="4" max="7"/>
-    <col width="12.77734375" customWidth="1" style="105" min="8" max="12"/>
-    <col width="12.77734375" customWidth="1" style="105" min="13" max="16384"/>
+    <col width="28" customWidth="1" style="106" min="1" max="1"/>
+    <col width="27.44140625" customWidth="1" style="106" min="2" max="2"/>
+    <col width="23.6640625" customWidth="1" style="106" min="3" max="3"/>
+    <col width="17.33203125" customWidth="1" style="106" min="4" max="7"/>
+    <col width="12.6640625" customWidth="1" style="106" min="8" max="12"/>
+    <col width="12.6640625" customWidth="1" style="106" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -35234,7 +35236,7 @@
           <t>Calcium supplementation</t>
         </is>
       </c>
-      <c r="B2" s="105" t="inlineStr">
+      <c r="B2" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35259,7 +35261,7 @@
       <c r="H2" s="74" t="n"/>
     </row>
     <row r="3">
-      <c r="C3" s="105" t="inlineStr">
+      <c r="C3" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35284,7 +35286,7 @@
           <t>Mg for pre-eclampsia</t>
         </is>
       </c>
-      <c r="B4" s="105" t="inlineStr">
+      <c r="B4" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35309,7 +35311,7 @@
       <c r="H4" s="83" t="n"/>
     </row>
     <row r="5">
-      <c r="C5" s="105" t="inlineStr">
+      <c r="C5" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35334,7 +35336,7 @@
           <t>Mg for eclampsia</t>
         </is>
       </c>
-      <c r="B6" s="105" t="inlineStr">
+      <c r="B6" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35359,7 +35361,7 @@
       <c r="H6" s="74" t="n"/>
     </row>
     <row r="7">
-      <c r="C7" s="105" t="inlineStr">
+      <c r="C7" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35424,7 +35426,7 @@
           <t>Calcium supplementation</t>
         </is>
       </c>
-      <c r="B11" s="105" t="inlineStr">
+      <c r="B11" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35452,7 +35454,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="C12" s="105" t="inlineStr">
+      <c r="C12" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35480,7 +35482,7 @@
           <t>Mg for pre-eclampsia</t>
         </is>
       </c>
-      <c r="B13" s="105" t="inlineStr">
+      <c r="B13" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35508,7 +35510,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="105" t="inlineStr">
+      <c r="C14" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35536,7 +35538,7 @@
           <t>Mg for eclampsia</t>
         </is>
       </c>
-      <c r="B15" s="105" t="inlineStr">
+      <c r="B15" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35564,7 +35566,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="105" t="inlineStr">
+      <c r="C16" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35632,7 +35634,7 @@
           <t>Calcium supplementation</t>
         </is>
       </c>
-      <c r="B20" s="105" t="inlineStr">
+      <c r="B20" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35660,7 +35662,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="105" t="inlineStr">
+      <c r="C21" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35688,7 +35690,7 @@
           <t>Mg for pre-eclampsia</t>
         </is>
       </c>
-      <c r="B22" s="105" t="inlineStr">
+      <c r="B22" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35716,7 +35718,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="105" t="inlineStr">
+      <c r="C23" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35744,7 +35746,7 @@
           <t>Mg for eclampsia</t>
         </is>
       </c>
-      <c r="B24" s="105" t="inlineStr">
+      <c r="B24" s="106" t="inlineStr">
         <is>
           <t>Hypertensive disorders</t>
         </is>
@@ -35772,7 +35774,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="C25" s="105" t="inlineStr">
+      <c r="C25" s="106" t="inlineStr">
         <is>
           <t>Effectiveness mortality</t>
         </is>
@@ -35808,8 +35810,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -35954,7 +35956,7 @@
       <c r="H12" s="12" t="n"/>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="2">
-      <c r="A13" s="105" t="inlineStr">
+      <c r="A13" s="106" t="inlineStr">
         <is>
           <t>Children</t>
         </is>
@@ -36315,6 +36317,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="A4pmOMTA42EFnc+7auattg==" formatRows="1" sort="1" spinCount="100000" hashValue="9PQsvPLydO8ZUJjer2hQv05DOzLM0QGx7Q/XJ3E/VpDQQUGgQ7s0kHD/IeTIOOYV5juy1GIL2kUv04K2BWZSTQ=="/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" scale="69" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -36329,8 +36332,8 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -36386,19 +36389,19 @@
           <t>Normal (HAZ-score &gt; -1)</t>
         </is>
       </c>
-      <c r="C2" s="43" t="n">
+      <c r="C2" s="104" t="n">
         <v>0.6181769353857089</v>
       </c>
-      <c r="D2" s="43" t="n">
+      <c r="D2" s="104" t="n">
         <v>0.6181769353857089</v>
       </c>
-      <c r="E2" s="43" t="n">
+      <c r="E2" s="104" t="n">
         <v>0.5620149534214139</v>
       </c>
-      <c r="F2" s="43" t="n">
+      <c r="F2" s="104" t="n">
         <v>0.361033010644528</v>
       </c>
-      <c r="G2" s="43" t="n">
+      <c r="G2" s="104" t="n">
         <v>0.312073173008955</v>
       </c>
     </row>
@@ -36408,19 +36411,19 @@
           <t>Mild (HAZ-score between -2 and -1)</t>
         </is>
       </c>
-      <c r="C3" s="43" t="n">
+      <c r="C3" s="104" t="n">
         <v>0.207556677169546</v>
       </c>
-      <c r="D3" s="43" t="n">
+      <c r="D3" s="104" t="n">
         <v>0.207556677169546</v>
       </c>
-      <c r="E3" s="43" t="n">
+      <c r="E3" s="104" t="n">
         <v>0.235507876049595</v>
       </c>
-      <c r="F3" s="43" t="n">
+      <c r="F3" s="104" t="n">
         <v>0.270745227373555</v>
       </c>
-      <c r="G3" s="43" t="n">
+      <c r="G3" s="104" t="n">
         <v>0.280148910444463</v>
       </c>
     </row>
@@ -36495,19 +36498,19 @@
           <t>Normal (WHZ-score &gt; -1)</t>
         </is>
       </c>
-      <c r="C8" s="43" t="n">
+      <c r="C8" s="104" t="n">
         <v>0.6803826715135181</v>
       </c>
-      <c r="D8" s="43" t="n">
+      <c r="D8" s="104" t="n">
         <v>0.6803826715135181</v>
       </c>
-      <c r="E8" s="43" t="n">
+      <c r="E8" s="104" t="n">
         <v>0.67220902049633</v>
       </c>
-      <c r="F8" s="43" t="n">
+      <c r="F8" s="104" t="n">
         <v>0.660936107781758</v>
       </c>
-      <c r="G8" s="43" t="n">
+      <c r="G8" s="104" t="n">
         <v>0.693194004191745</v>
       </c>
     </row>
@@ -36517,19 +36520,19 @@
           <t>Mild (WHZ-score between -2 and -1)</t>
         </is>
       </c>
-      <c r="C9" s="43" t="n">
+      <c r="C9" s="104" t="n">
         <v>0.183806055435209</v>
       </c>
-      <c r="D9" s="43" t="n">
+      <c r="D9" s="104" t="n">
         <v>0.183806055435209</v>
       </c>
-      <c r="E9" s="43" t="n">
+      <c r="E9" s="104" t="n">
         <v>0.199612128157314</v>
       </c>
-      <c r="F9" s="43" t="n">
+      <c r="F9" s="104" t="n">
         <v>0.220254269533283</v>
       </c>
-      <c r="G9" s="43" t="n">
+      <c r="G9" s="104" t="n">
         <v>0.223042336282145</v>
       </c>
     </row>
@@ -36592,7 +36595,7 @@
       <c r="O12" s="5" t="n"/>
     </row>
     <row r="13" ht="27" customHeight="1" s="2">
-      <c r="A13" s="105" t="inlineStr">
+      <c r="A13" s="106" t="inlineStr">
         <is>
           <t>Anaemia</t>
         </is>
@@ -36715,34 +36718,57 @@
           <t>Prevalence of iron deficiency anaemia</t>
         </is>
       </c>
-      <c r="C15" s="43" t="n"/>
-      <c r="D15" s="43" t="n"/>
-      <c r="E15" s="43" t="n"/>
-      <c r="F15" s="43" t="n"/>
-      <c r="G15" s="43" t="n"/>
-      <c r="H15" s="43" t="n">
-        <v>0.185580948</v>
-      </c>
-      <c r="I15" s="43" t="n">
-        <v>0.185580948</v>
-      </c>
-      <c r="J15" s="43" t="n">
-        <v>0.185580948</v>
-      </c>
-      <c r="K15" s="43" t="n">
-        <v>0.185580948</v>
-      </c>
-      <c r="L15" s="43" t="n">
-        <v>0.1913512</v>
-      </c>
-      <c r="M15" s="43" t="n">
-        <v>0.1913512</v>
-      </c>
-      <c r="N15" s="43" t="n">
-        <v>0.1913512</v>
-      </c>
-      <c r="O15" s="43" t="n">
-        <v>0.1913512</v>
+      <c r="C15" s="43">
+        <f>C14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="D15" s="43">
+        <f>D14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="E15" s="43">
+        <f>E14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="F15" s="43">
+        <f>F14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="G15" s="43">
+        <f>G14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="H15" s="43">
+        <f>H14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="I15" s="43">
+        <f>I14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="J15" s="43">
+        <f>J14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="K15" s="43">
+        <f>K14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="L15" s="43">
+        <f>L14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="M15" s="43">
+        <f>M14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="N15" s="43">
+        <f>N14*iron_deficiency_anaemia</f>
+        <v/>
+      </c>
+      <c r="O15" s="43">
+        <f>O14*iron_deficiency_anaemia</f>
+        <v/>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="2">
@@ -36760,6 +36786,7 @@
       <c r="G17" s="3" t="n"/>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="+8OS651lS1+nSfe4CulhMw==" formatRows="1" sort="1" spinCount="100000" hashValue="hxDW4htzQBx7GiuMXHCW2YMPpttA3FrJFsUvngy5BORqU3YtEBb+/75LGdy+1cPxGGZOeHr/l3RmBqsiEScXng=="/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -36775,7 +36802,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -36794,27 +36821,27 @@
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="105" t="inlineStr">
+      <c r="C1" s="106" t="inlineStr">
         <is>
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="D1" s="105" t="inlineStr">
+      <c r="D1" s="106" t="inlineStr">
         <is>
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="E1" s="105" t="inlineStr">
+      <c r="E1" s="106" t="inlineStr">
         <is>
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="F1" s="105" t="inlineStr">
+      <c r="F1" s="106" t="inlineStr">
         <is>
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="G1" s="105" t="inlineStr">
+      <c r="G1" s="106" t="inlineStr">
         <is>
           <t>24-59 months</t>
         </is>
@@ -36837,9 +36864,15 @@
       <c r="D2" s="44" t="n">
         <v>0.4193781</v>
       </c>
-      <c r="E2" s="44" t="n"/>
-      <c r="F2" s="44" t="n"/>
-      <c r="G2" s="44" t="n"/>
+      <c r="E2" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="83" t="inlineStr">
@@ -36853,9 +36886,15 @@
       <c r="D3" s="44" t="n">
         <v>0.1167952</v>
       </c>
-      <c r="E3" s="44" t="n"/>
-      <c r="F3" s="44" t="n"/>
-      <c r="G3" s="44" t="n"/>
+      <c r="E3" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="83" t="inlineStr">
@@ -36875,7 +36914,9 @@
       <c r="F4" s="44" t="n">
         <v>0.738078653812408</v>
       </c>
-      <c r="G4" s="44" t="n"/>
+      <c r="G4" s="44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="83" t="inlineStr">
@@ -36883,22 +36924,25 @@
           <t>None</t>
         </is>
       </c>
-      <c r="C5" s="43" t="n">
+      <c r="C5" s="104" t="n">
         <v>0.0171813070774078</v>
       </c>
-      <c r="D5" s="43" t="n">
+      <c r="D5" s="104" t="n">
         <v>0.0379721000000001</v>
       </c>
-      <c r="E5" s="43" t="n">
+      <c r="E5" s="104" t="n">
         <v>0.09623706340789795</v>
       </c>
-      <c r="F5" s="43" t="n">
+      <c r="F5" s="104" t="n">
         <v>0.261921346187592</v>
       </c>
-      <c r="G5" s="43" t="n"/>
+      <c r="G5" s="104">
+        <f>1-SUM(G2:G4)</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="TyxzFz+E2uI3dTroZBTeAA==" formatRows="1" sort="1" spinCount="100000" hashValue="cjZGG35skIN/87gVYPq+qku8px1GpcfbcC9VQGwmKjtdbvNEf7x1kHTHwQlPZMuOorjL/9FyNZdN8JPWk+p31Q=="/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="DWOkVPLBaYjCNLYsICz9ww==" formatRows="1" sort="1" spinCount="100000" hashValue="KVM6fA8r70knWIZGz+ZsotJ9UbI6hUI/7Ufd/oa5vsEdb+fMLF4sjVnHmH8N4IGnGTY1AvsNGXWfuffGvzQssw=="/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
@@ -36986,36 +37030,16 @@
           <t>Children 0-59 months</t>
         </is>
       </c>
-      <c r="C2" s="15" t="n">
-        <v>0.48186</v>
-      </c>
-      <c r="D2" s="15" t="n">
-        <v>0.47707</v>
-      </c>
-      <c r="E2" s="15" t="n">
-        <v>0.47232</v>
-      </c>
-      <c r="F2" s="15" t="n">
-        <v>0.46767</v>
-      </c>
-      <c r="G2" s="15" t="n">
-        <v>0.46308</v>
-      </c>
-      <c r="H2" s="15" t="n">
-        <v>0.45862</v>
-      </c>
-      <c r="I2" s="15" t="n">
-        <v>0.45427</v>
-      </c>
-      <c r="J2" s="15" t="n">
-        <v>0.44997</v>
-      </c>
-      <c r="K2" s="15" t="n">
-        <v>0.44567</v>
-      </c>
-      <c r="L2" s="15" t="n">
-        <v>0.44137</v>
-      </c>
+      <c r="C2" s="15" t="n"/>
+      <c r="D2" s="15" t="n"/>
+      <c r="E2" s="15" t="n"/>
+      <c r="F2" s="15" t="n"/>
+      <c r="G2" s="15" t="n"/>
+      <c r="H2" s="15" t="n"/>
+      <c r="I2" s="15" t="n"/>
+      <c r="J2" s="15" t="n"/>
+      <c r="K2" s="15" t="n"/>
+      <c r="L2" s="15" t="n"/>
     </row>
     <row r="3">
       <c r="B3" s="19" t="n"/>
@@ -37031,36 +37055,16 @@
           <t>Children 0-59 months</t>
         </is>
       </c>
-      <c r="C4" s="15" t="n">
-        <v>0.04398</v>
-      </c>
-      <c r="D4" s="15" t="n">
-        <v>0.04283000000000001</v>
-      </c>
-      <c r="E4" s="15" t="n">
-        <v>0.04171</v>
-      </c>
-      <c r="F4" s="15" t="n">
-        <v>0.04063</v>
-      </c>
-      <c r="G4" s="15" t="n">
-        <v>0.03957</v>
-      </c>
-      <c r="H4" s="15" t="n">
-        <v>0.03854</v>
-      </c>
-      <c r="I4" s="15" t="n">
-        <v>0.03754</v>
-      </c>
-      <c r="J4" s="15" t="n">
-        <v>0.03656</v>
-      </c>
-      <c r="K4" s="15" t="n">
-        <v>0.03563</v>
-      </c>
-      <c r="L4" s="15" t="n">
-        <v>0.03473</v>
-      </c>
+      <c r="C4" s="15" t="n"/>
+      <c r="D4" s="15" t="n"/>
+      <c r="E4" s="15" t="n"/>
+      <c r="F4" s="15" t="n"/>
+      <c r="G4" s="15" t="n"/>
+      <c r="H4" s="15" t="n"/>
+      <c r="I4" s="15" t="n"/>
+      <c r="J4" s="15" t="n"/>
+      <c r="K4" s="15" t="n"/>
+      <c r="L4" s="15" t="n"/>
     </row>
     <row r="5">
       <c r="B5" s="19" t="n"/>
@@ -37161,7 +37165,7 @@
       <c r="L11" s="15" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="105" t="inlineStr">
+      <c r="A13" s="106" t="inlineStr">
         <is>
           <t>Mortality</t>
         </is>
@@ -37171,36 +37175,16 @@
           <t>Under five (deaths per 1,000 births)</t>
         </is>
       </c>
-      <c r="C13" s="103" t="n">
-        <v>47.447</v>
-      </c>
-      <c r="D13" s="103" t="n">
-        <v>46.053</v>
-      </c>
-      <c r="E13" s="103" t="n">
-        <v>44.578</v>
-      </c>
-      <c r="F13" s="103" t="n">
-        <v>43.29</v>
-      </c>
-      <c r="G13" s="103" t="n">
-        <v>42.021</v>
-      </c>
-      <c r="H13" s="103" t="n">
-        <v>40.637</v>
-      </c>
-      <c r="I13" s="103" t="n">
-        <v>41.034</v>
-      </c>
-      <c r="J13" s="103" t="n">
-        <v>38.126</v>
-      </c>
-      <c r="K13" s="103" t="n">
-        <v>37.522</v>
-      </c>
-      <c r="L13" s="103" t="n">
-        <v>36.866</v>
-      </c>
+      <c r="C13" s="102" t="n"/>
+      <c r="D13" s="102" t="n"/>
+      <c r="E13" s="102" t="n"/>
+      <c r="F13" s="102" t="n"/>
+      <c r="G13" s="102" t="n"/>
+      <c r="H13" s="102" t="n"/>
+      <c r="I13" s="102" t="n"/>
+      <c r="J13" s="102" t="n"/>
+      <c r="K13" s="102" t="n"/>
+      <c r="L13" s="102" t="n"/>
     </row>
     <row r="14">
       <c r="B14" s="70" t="inlineStr">
@@ -37208,16 +37192,16 @@
           <t>Maternal (deaths per 1,000 births)</t>
         </is>
       </c>
-      <c r="C14" s="103" t="n"/>
-      <c r="D14" s="103" t="n"/>
-      <c r="E14" s="103" t="n"/>
-      <c r="F14" s="103" t="n"/>
-      <c r="G14" s="103" t="n"/>
-      <c r="H14" s="103" t="n"/>
-      <c r="I14" s="103" t="n"/>
-      <c r="J14" s="103" t="n"/>
-      <c r="K14" s="103" t="n"/>
-      <c r="L14" s="103" t="n"/>
+      <c r="C14" s="102" t="n"/>
+      <c r="D14" s="102" t="n"/>
+      <c r="E14" s="102" t="n"/>
+      <c r="F14" s="102" t="n"/>
+      <c r="G14" s="102" t="n"/>
+      <c r="H14" s="102" t="n"/>
+      <c r="I14" s="102" t="n"/>
+      <c r="J14" s="102" t="n"/>
+      <c r="K14" s="102" t="n"/>
+      <c r="L14" s="102" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37235,7 +37219,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -37257,66 +37241,67 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="105" t="inlineStr">
+      <c r="A2" s="106" t="inlineStr">
         <is>
           <t>Child wasting episode</t>
         </is>
       </c>
-      <c r="B2" s="99" t="n">
+      <c r="B2" s="32" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="105" t="inlineStr">
+      <c r="A3" s="106" t="inlineStr">
         <is>
           <t>Child turning age 5 stunted (over lifetime)</t>
         </is>
       </c>
-      <c r="B3" s="99" t="n">
+      <c r="B3" s="32" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="105" t="inlineStr">
+      <c r="A4" s="106" t="inlineStr">
         <is>
           <t>Child death</t>
         </is>
       </c>
-      <c r="B4" s="99" t="n">
-        <v>50</v>
+      <c r="B4" s="32" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="105" t="inlineStr">
+      <c r="A5" s="106" t="inlineStr">
         <is>
           <t>Maternal death</t>
         </is>
       </c>
-      <c r="B5" s="99" t="n">
-        <v>100</v>
+      <c r="B5" s="32" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="105" t="inlineStr">
+      <c r="A6" s="106" t="inlineStr">
         <is>
           <t>Anaemic child (per year)</t>
         </is>
       </c>
-      <c r="B6" s="99" t="n">
-        <v>5</v>
+      <c r="B6" s="32" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="105" t="inlineStr">
+      <c r="A7" s="106" t="inlineStr">
         <is>
           <t>Anaemic pregnant woman (per pregnancy)</t>
         </is>
       </c>
-      <c r="B7" s="99" t="n">
-        <v>5</v>
+      <c r="B7" s="32" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="AE9JYpQ3KeQ6lUhqrRhxOQ==" formatRows="1" sort="1" spinCount="100000" hashValue="rY4IEhIq3lEn09wA9WriBN7WGsc6Nw25jW0hwf10pL82OGICKDMyc7PpnwW2SYWlxF3aQoaG8LP4NxR5RvcRIw=="/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -37336,11 +37321,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col width="17" customWidth="1" style="105" min="1" max="1"/>
-    <col width="19.109375" customWidth="1" style="105" min="2" max="2"/>
-    <col width="13.44140625" customWidth="1" style="105" min="3" max="3"/>
-    <col width="11.44140625" customWidth="1" style="105" min="4" max="8"/>
-    <col width="11.44140625" customWidth="1" style="105" min="9" max="16384"/>
+    <col width="17" customWidth="1" style="106" min="1" max="1"/>
+    <col width="19.109375" customWidth="1" style="106" min="2" max="2"/>
+    <col width="13.44140625" customWidth="1" style="106" min="3" max="3"/>
+    <col width="11.44140625" customWidth="1" style="106" min="4" max="8"/>
+    <col width="11.44140625" customWidth="1" style="106" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -37394,10 +37379,12 @@
           <t>&lt;1 month</t>
         </is>
       </c>
-      <c r="C3" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="47" t="n"/>
+      <c r="C3" s="47" t="n"/>
+      <c r="D3" s="47" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E3" s="29">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -37409,10 +37396,12 @@
           <t>1-5 months</t>
         </is>
       </c>
-      <c r="C4" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="47" t="n"/>
+      <c r="C4" s="47" t="n"/>
+      <c r="D4" s="47" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E4" s="29">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -37424,9 +37413,7 @@
           <t>6-11 months</t>
         </is>
       </c>
-      <c r="C5" s="47" t="b">
-        <v>1</v>
-      </c>
+      <c r="C5" s="47" t="n"/>
       <c r="D5" s="47" t="n"/>
       <c r="E5" s="29">
         <f>IF(E$7="","",E$7)</f>
@@ -37439,9 +37426,7 @@
           <t>12-23 months</t>
         </is>
       </c>
-      <c r="C6" s="47" t="b">
-        <v>1</v>
-      </c>
+      <c r="C6" s="47" t="n"/>
       <c r="D6" s="47" t="n"/>
       <c r="E6" s="29">
         <f>IF(E$7="","",E$7)</f>
@@ -37470,9 +37455,7 @@
         </is>
       </c>
       <c r="C9" s="47" t="n"/>
-      <c r="D9" s="47" t="b">
-        <v>0</v>
-      </c>
+      <c r="D9" s="47" t="n"/>
       <c r="E9" s="29">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -37511,7 +37494,11 @@
         </is>
       </c>
       <c r="C12" s="47" t="n"/>
-      <c r="D12" s="47" t="n"/>
+      <c r="D12" s="47" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E12" s="29">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -37524,7 +37511,11 @@
         </is>
       </c>
       <c r="C13" s="47" t="n"/>
-      <c r="D13" s="47" t="n"/>
+      <c r="D13" s="47" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E13" s="29">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -37538,11 +37529,7 @@
       </c>
       <c r="C14" s="23" t="n"/>
       <c r="D14" s="22" t="n"/>
-      <c r="E14" s="47" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="E14" s="47" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="26" t="inlineStr">

</xml_diff>